<commit_message>
including two digits days
</commit_message>
<xml_diff>
--- a/ICU_6.xlsx
+++ b/ICU_6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -88,6 +88,9 @@
     <t>松井貴裕</t>
   </si>
   <si>
+    <t>松原龍輔</t>
+  </si>
+  <si>
     <t>松永崇宏</t>
   </si>
   <si>
@@ -106,6 +109,9 @@
     <t>清水　隆之</t>
   </si>
   <si>
+    <t>熊木聡美</t>
+  </si>
+  <si>
     <t>片山充哉</t>
   </si>
   <si>
@@ -166,97 +172,115 @@
     <t>髙木菜々美</t>
   </si>
   <si>
-    <t>6月4日 ,6月6日</t>
-  </si>
-  <si>
-    <t>6月2日 ,6月3日 ,6月4日 ,6月6日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月6日 ,6月7日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月3日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月6日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日 ,6月4日 ,6月5日 ,6月7日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月7日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月2日 ,6月3日 ,6月5日 ,6月6日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日 ,6月3日 ,6月5日 ,6月6日 ,6月7日</t>
+    <t>6月4日 ,6月6日 ,6月11日 ,6月13日 ,6月18日 ,6月20日 ,6月25日 ,6月27日</t>
+  </si>
+  <si>
+    <t>6月2日 ,6月3日 ,6月4日 ,6月6日 ,6月9日 ,6月10日 ,6月11日 ,6月13日 ,6月16日 ,6月17日 ,6月18日 ,6月20日 ,6月23日 ,6月24日 ,6月25日 ,6月27日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月6日 ,6月7日 ,6月8日 ,6月9日 ,6月10日 ,6月11日 ,6月13日 ,6月14日 ,6月17日 ,6月18日 ,6月20日 ,6月21日 ,6月24日 ,6月25日 ,6月27日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月3日 ,6月16日 ,6月17日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月11日 ,6月12日 ,6月13日 ,6月16日 ,6月17日 ,6月18日 ,6月19日 ,6月20日 ,6月23日 ,6月24日 ,6月25日 ,6月26日 ,6月27日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月4日 ,6月5日 ,6月7日 ,6月8日 ,6月9日 ,6月11日 ,6月12日 ,6月14日 ,6月15日 ,6月16日 ,6月18日 ,6月19日 ,6月25日 ,6月26日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月7日 ,6月8日 ,6月9日 ,6月10日 ,6月11日 ,6月12日 ,6月13日 ,6月14日 ,6月17日 ,6月18日 ,6月19日 ,6月20日 ,6月21日 ,6月22日 ,6月23日 ,6月24日 ,6月25日 ,6月26日 ,6月27日 ,6月28日</t>
+  </si>
+  <si>
+    <t>6月2日 ,6月3日 ,6月5日 ,6月6日 ,6月10日 ,6月12日 ,6月13日 ,6月15日 ,6月17日 ,6月20日 ,6月24日 ,6月26日 ,6月27日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月3日 ,6月5日 ,6月6日 ,6月7日 ,6月10日 ,6月12日 ,6月13日 ,6月14日 ,6月15日 ,6月16日 ,6月17日 ,6月19日 ,6月20日 ,6月21日 ,6月22日 ,6月23日 ,6月24日 ,6月26日 ,6月27日</t>
   </si>
   <si>
     <t>6月4日 (火) ,6月5日 (水) ,6月11日 (火) ,6月12日 (水) ,6月14日 (金) ,6月18日 (火) ,6月19日 (水) ,6月25日 (火) ,6月26日 (水) ,6月27日 (木) ,6月28日 (金)</t>
   </si>
   <si>
-    <t>6月8日</t>
-  </si>
-  <si>
-    <t>6月4日 ,6月5日 ,6月6日 ,6月7日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月2日 ,6月5日 ,6月6日 ,6月7日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日</t>
-  </si>
-  <si>
-    <t>6月1日</t>
-  </si>
-  <si>
-    <t>6月3日 ,6月5日 ,6月7日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月5日 ,6月7日 ,6月8日</t>
-  </si>
-  <si>
-    <t>6月9日</t>
-  </si>
-  <si>
-    <t>6月5日</t>
-  </si>
-  <si>
-    <t>6月5日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日 ,6月5日 ,6月7日 ,6月8日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月6日 ,6月7日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月6日 ,6月7日 ,6月8日</t>
+    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月6日 ,6月7日 ,6月8日 ,6月9日 ,6月10日 ,6月11日 ,6月13日 ,6月14日 ,6月16日 ,6月17日 ,6月18日 ,6月20日 ,6月21日 ,6月23日 ,6月24日 ,6月25日 ,6月27日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月8日 ,6月22日</t>
+  </si>
+  <si>
+    <t>6月4日 ,6月5日 ,6月6日 ,6月7日 ,6月8日 ,6月9日 ,6月10日 ,6月11日 ,6月12日 ,6月13日 ,6月14日 ,6月15日 ,6月16日 ,6月17日 ,6月18日 ,6月19日 ,6月20日 ,6月21日 ,6月22日 ,6月23日 ,6月24日 ,6月25日 ,6月26日 ,6月27日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月2日 ,6月5日 ,6月6日 ,6月7日 ,6月9日 ,6月11日 ,6月12日 ,6月13日 ,6月14日 ,6月19日 ,6月20日 ,6月21日 ,6月23日 ,6月26日 ,6月27日 ,6月28日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月22日 ,6月23日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月14日 ,6月21日 ,6月28日</t>
+  </si>
+  <si>
+    <t>6月3日 ,6月5日 ,6月7日 ,6月8日 ,6月9日 ,6月10日 ,6月12日 ,6月17日 ,6月19日 ,6月21日 ,6月22日 ,6月23日 ,6月24日 ,6月26日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月5日 ,6月7日 ,6月8日 ,6月12日 ,6月14日 ,6月15日 ,6月19日 ,6月21日 ,6月22日 ,6月26日 ,6月28日 ,6月29日</t>
+  </si>
+  <si>
+    <t>6月8日 ,6月14日 ,6月15日 ,6月16日</t>
+  </si>
+  <si>
+    <t>6月9日 ,6月16日 ,6月23日 ,6月27日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月7日 ,6月8日 ,6月9日 ,6月10日 ,6月11日 ,6月12日 ,6月13日 ,6月14日 ,6月15日 ,6月16日 ,6月17日 ,6月18日 ,6月19日 ,6月20日 ,6月21日 ,6月22日 ,6月23日 ,6月24日 ,6月25日 ,6月26日 ,6月27日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月5日 ,6月12日 ,6月15日 ,6月16日 ,6月19日 ,6月22日 ,6月23日 ,6月26日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月15日 ,6月16日 ,6月29日</t>
+  </si>
+  <si>
+    <t>6月5日 ,6月8日 ,6月9日 ,6月12日 ,6月18日 ,6月19日 ,6月22日 ,6月23日 ,6月26日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月5日 ,6月7日 ,6月8日 ,6月12日 ,6月19日 ,6月21日 ,6月22日 ,6月26日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月6日 ,6月7日 ,6月8日 ,6月9日 ,6月11日 ,6月12日 ,6月13日 ,6月20日 ,6月21日 ,6月22日 ,6月23日 ,6月25日 ,6月26日 ,6月27日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月6日 ,6月7日 ,6月8日 ,6月15日 ,6月21日 ,6月22日 ,6月23日 ,6月28日 ,6月29日</t>
   </si>
   <si>
     <t>6月６日 (木) ,6月7日 (金) ,6月8日 (土) ,6月14日 (金) ,6月21日 (金) ,6月28日 (金) ,6月29日 (土) ,6月30日 (日)</t>
   </si>
   <si>
-    <t>6月7日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月3日 ,6月6日</t>
-  </si>
-  <si>
-    <t>6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月7日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月2日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月2日 ,6月4日 ,6月5日 ,6月6日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月7日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月4日 ,6月8日 ,6月9日</t>
+    <t>6月7日 ,6月8日 ,6月9日 ,6月10日 ,6月14日 ,6月15日 ,6月21日 ,6月22日</t>
+  </si>
+  <si>
+    <t>6月3日 ,6月6日 ,6月10日 ,6月13日 ,6月17日 ,6月20日 ,6月21日 ,6月22日 ,6月23日 ,6月24日 ,6月27日</t>
+  </si>
+  <si>
+    <t>6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月7日 ,6月9日 ,6月10日 ,6月11日 ,6月12日 ,6月14日 ,6月15日 ,6月16日 ,6月17日 ,6月18日 ,6月19日 ,6月23日 ,6月24日 ,6月25日 ,6月26日 ,6月27日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月2日 ,6月9日 ,6月16日 ,6月22日 ,6月23日 ,6月24日 ,6月25日 ,6月26日 ,6月27日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月15日 ,6月16日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月2日 ,6月4日 ,6月5日 ,6月6日 ,6月9日 ,6月10日 ,6月12日 ,6月13日 ,6月16日 ,6月19日 ,6月20日 ,6月23日 ,6月26日 ,6月27日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月7日 ,6月8日 ,6月9日 ,6月16日 ,6月19日 ,6月21日 ,6月22日 ,6月23日 ,6月29日</t>
+  </si>
+  <si>
+    <t>6月4日 ,6月8日 ,6月9日 ,6月11日 ,6月18日 ,6月25日 ,6月28日 ,6月29日 ,6月30日</t>
   </si>
   <si>
     <t>6月1日 (土) ,6月3日 (月) ,6月7日 (金) ,6月8日 (土) ,6月10日 (月) ,6月17日 (月) ,6月20日 (木) ,6月21日 (金) ,6月22日 (土) ,6月24日 (月)</t>
@@ -265,55 +289,67 @@
     <t>6月1日 (土) ,6月2日 (日) ,6月8日 (土) ,6月15日 (土) ,6月16日 (日)</t>
   </si>
   <si>
-    <t>6月4日</t>
-  </si>
-  <si>
-    <t>6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月7日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日 ,6月7日 ,6月8日</t>
-  </si>
-  <si>
-    <t>6月3日 ,6月5日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月7日 ,6月8日</t>
+    <t>6月5日 ,6月12日 ,6月15日 ,6月19日 ,6月22日 ,6月26日</t>
+  </si>
+  <si>
+    <t>6月17日</t>
+  </si>
+  <si>
+    <t>6月4日 ,6月11日 ,6月18日 ,6月25日</t>
+  </si>
+  <si>
+    <t>6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月7日 ,6月10日 ,6月11日 ,6月12日 ,6月13日 ,6月14日 ,6月15日 ,6月16日 ,6月17日 ,6月18日 ,6月19日 ,6月20日 ,6月21日 ,6月23日 ,6月24日 ,6月25日 ,6月26日 ,6月27日 ,6月28日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月7日 ,6月8日 ,6月14日 ,6月15日 ,6月21日 ,6月22日 ,6月28日 ,6月29日</t>
+  </si>
+  <si>
+    <t>6月3日 ,6月5日 ,6月10日 ,6月12日 ,6月14日 ,6月15日 ,6月16日 ,6月17日 ,6月19日 ,6月24日 ,6月26日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月4日 ,6月8日 ,6月9日 ,6月11日 ,6月18日 ,6月25日 ,6月26日 ,6月27日 ,6月28日 ,6月29日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月7日 ,6月8日 ,6月14日 ,6月15日</t>
   </si>
   <si>
     <t>6月1日 (土) ,6月2日 (日) ,6月3日 (月) ,6月15日 (土) ,6月16日 (日)</t>
   </si>
   <si>
-    <t>6月1日 ,6月2日 ,6月4日</t>
+    <t>6月1日 ,6月2日 ,6月4日 ,6月11日 ,6月15日 ,6月18日 ,6月25日 ,6月28日 ,6月29日 ,6月30日</t>
   </si>
   <si>
     <t>6月1日 (土) ,6月5日 (水) ,6月7日 (金) ,6月8日 (土) ,6月12日 (水) ,6月16日 (日) ,6月18日 (火) ,6月19日 (水) ,6月26日 (水) ,6月29日 (土)</t>
   </si>
   <si>
-    <t>6月4日 ,6月5日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月2日 ,6月5日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月1日 ,6月2日 ,6月4日 ,6月8日 ,6月9日</t>
+    <t>6月4日 ,6月5日 ,6月11日 ,6月12日 ,6月18日 ,6月19日 ,6月21日 ,6月22日 ,6月23日 ,6月25日 ,6月26日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月3日 ,6月4日 ,6月8日 ,6月9日 ,6月10日 ,6月11日 ,6月16日 ,6月17日 ,6月18日 ,6月23日 ,6月24日 ,6月25日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月2日 ,6月5日 ,6月9日 ,6月11日 ,6月12日 ,6月16日 ,6月19日 ,6月23日 ,6月26日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月1日 ,6月2日 ,6月4日 ,6月8日 ,6月9日 ,6月11日 ,6月18日 ,6月22日 ,6月25日 ,6月29日</t>
   </si>
   <si>
     <t>6月7日 ,6月8日</t>
   </si>
   <si>
+    <t>6月1日 ,6月2日 ,6月15日 ,6月16日</t>
+  </si>
+  <si>
     <t>6月1日 ,6月2日 ,6月3日</t>
   </si>
   <si>
-    <t>6月1日 ,6月3日 ,6月4日 ,6月8日</t>
-  </si>
-  <si>
-    <t>6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月8日 ,6月9日</t>
-  </si>
-  <si>
-    <t>6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月7日 ,6月8日 ,6月9日</t>
+    <t>6月1日 ,6月3日 ,6月4日 ,6月8日 ,6月10日 ,6月15日 ,6月16日 ,6月17日 ,6月18日 ,6月22日 ,6月24日 ,6月25日 ,6月29日</t>
+  </si>
+  <si>
+    <t>6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月8日 ,6月9日 ,6月10日 ,6月11日 ,6月12日 ,6月13日 ,6月14日 ,6月15日 ,6月16日 ,6月17日 ,6月18日 ,6月19日 ,6月20日 ,6月21日 ,6月24日 ,6月25日 ,6月26日 ,6月27日 ,6月28日 ,6月29日 ,6月30日</t>
+  </si>
+  <si>
+    <t>6月2日 ,6月3日 ,6月4日 ,6月5日 ,6月6日 ,6月7日 ,6月8日 ,6月9日 ,6月10日 ,6月11日 ,6月12日 ,6月13日 ,6月15日 ,6月16日 ,6月17日 ,6月18日 ,6月19日 ,6月20日 ,6月22日 ,6月23日 ,6月24日 ,6月25日 ,6月26日 ,6月27日 ,6月29日 ,6月30日</t>
   </si>
   <si>
     <t>6月1日 ,6月2日 ,6月9日</t>
@@ -702,7 +738,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -733,13 +769,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -750,13 +786,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -767,10 +803,10 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -781,10 +817,10 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -795,13 +831,13 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -812,13 +848,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -829,13 +865,13 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -846,10 +882,10 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -860,10 +896,10 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -874,16 +910,16 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F11" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -894,10 +930,10 @@
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -908,10 +944,10 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -922,13 +958,13 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -939,10 +975,10 @@
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -953,13 +989,13 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -970,16 +1006,16 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -990,10 +1026,10 @@
         <v>21</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1004,10 +1040,10 @@
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1018,10 +1054,13 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>84</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1032,10 +1071,10 @@
         <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1045,17 +1084,11 @@
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" t="s">
-        <v>57</v>
-      </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1066,16 +1099,16 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F23" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1086,13 +1119,16 @@
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>113</v>
+      </c>
+      <c r="F24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1102,11 +1138,14 @@
       <c r="B25" t="s">
         <v>28</v>
       </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1116,14 +1155,11 @@
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C26" t="s">
-        <v>52</v>
-      </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1133,11 +1169,14 @@
       <c r="B27" t="s">
         <v>30</v>
       </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1148,10 +1187,10 @@
         <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1162,10 +1201,10 @@
         <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1175,14 +1214,11 @@
       <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C30" t="s">
-        <v>60</v>
-      </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1193,10 +1229,10 @@
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E31" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1206,11 +1242,14 @@
       <c r="B32" t="s">
         <v>35</v>
       </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1221,10 +1260,10 @@
         <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1235,10 +1274,10 @@
         <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1249,10 +1288,10 @@
         <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1263,10 +1302,10 @@
         <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E36" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1277,10 +1316,10 @@
         <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1291,13 +1330,10 @@
         <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E38" t="s">
-        <v>101</v>
-      </c>
-      <c r="F38" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1308,10 +1344,10 @@
         <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E39" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1322,10 +1358,13 @@
         <v>43</v>
       </c>
       <c r="D40" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E40" t="s">
-        <v>101</v>
+        <v>113</v>
+      </c>
+      <c r="F40" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1336,10 +1375,10 @@
         <v>44</v>
       </c>
       <c r="D41" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1349,14 +1388,11 @@
       <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="C42" t="s">
-        <v>61</v>
-      </c>
       <c r="D42" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E42" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1366,14 +1402,11 @@
       <c r="B43" t="s">
         <v>46</v>
       </c>
-      <c r="C43" t="s">
-        <v>62</v>
-      </c>
       <c r="D43" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E43" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1384,13 +1417,13 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="E44" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1401,13 +1434,13 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1417,11 +1450,45 @@
       <c r="B46" t="s">
         <v>49</v>
       </c>
+      <c r="C46" t="s">
+        <v>66</v>
+      </c>
       <c r="D46" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E46" t="s">
-        <v>101</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>